<commit_message>
Toevoeging van opleidingsvormen en buitengewoon onderwijs.
</commit_message>
<xml_diff>
--- a/ilearn/onderwijsstructuur-extension/input/onderwijsstructuur.xlsx
+++ b/ilearn/onderwijsstructuur-extension/input/onderwijsstructuur.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="171">
   <si>
     <t xml:space="preserve">mapping</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">subniveau</t>
   </si>
   <si>
+    <t xml:space="preserve">opleidingsvorm</t>
+  </si>
+  <si>
     <t xml:space="preserve">graad</t>
   </si>
   <si>
@@ -70,6 +73,12 @@
     <t xml:space="preserve">onderwijs subniveaus</t>
   </si>
   <si>
+    <t xml:space="preserve">verzameling-opleidingsvorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opleidingsvormen</t>
+  </si>
+  <si>
     <t xml:space="preserve">verzameling-graad</t>
   </si>
   <si>
@@ -425,6 +434,81 @@
   </si>
   <si>
     <t xml:space="preserve">secundair 3e graad 3e leerjaar finaliteit arbeidsmarkt bso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon-basisonderwijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon basisonderwijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon-kleuteronderwijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon kleuteronderwijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon-lager-onderwijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon lager onderwijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon-secundair-onderwijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon secundair onderwijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opleidingsvorm-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opleidingsvorm 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opleidingsvorm-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opleidingsvorm 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opleidingsvorm-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opleidingsvorm 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opleidingsvorm-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opleidingsvorm 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graad-onder-opleidingsvorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon-secundair-1e-graad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon secundair 1e graad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon-secundair-2e-graad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon secundair 2e graad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon-secundair-3e-graad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon secundair 3e graad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon-secundair-3e-graad-3e-leerjaar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buitengewoon secundair 3e graad 3e leerjaar</t>
   </si>
   <si>
     <t xml:space="preserve">volwassenenonderwijs</t>
@@ -606,24 +690,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H75" activeCellId="0" sqref="H75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J64" activeCellId="0" sqref="J64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="36.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="36.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="36.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="43.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="47.02"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,210 +736,202 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B11" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="2" t="s">
         <v>30</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="K12" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>32</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>36</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -863,65 +940,65 @@
         <v>40</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="J17" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="K17" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>44</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>46</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -929,65 +1006,65 @@
         <v>40</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I20" s="2" t="s">
         <v>48</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>50</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="I22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,232 +1072,232 @@
         <v>40</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="2" t="s">
         <v>54</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="I24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>56</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="I25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>58</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="K26" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="0" t="s">
         <v>60</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="I27" s="2" t="s">
         <v>63</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="0" t="s">
         <v>60</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="I28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>65</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>60</v>
+        <v>60</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I29" s="2" t="s">
         <v>67</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="K29" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="K31" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="I32" s="2" t="s">
         <v>75</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="I33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>77</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I34" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>79</v>
       </c>
       <c r="J34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K34" s="2" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1229,87 +1306,87 @@
         <v>7</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>78</v>
+        <v>60</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="H35" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="J35" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>78</v>
+        <v>60</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="H36" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I36" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="J36" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>78</v>
+        <v>60</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="H37" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I37" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="J37" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="K37" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G38" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I38" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="J38" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1318,64 +1395,64 @@
         <v>7</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>90</v>
+        <v>60</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="H39" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="J39" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="K39" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>90</v>
+        <v>60</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="I40" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>96</v>
+      <c r="K40" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="I41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="I41" s="0" t="s">
         <v>98</v>
       </c>
       <c r="J41" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K41" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1384,99 +1461,99 @@
         <v>7</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>97</v>
+        <v>60</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="H42" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="J42" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="K42" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I43" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>104</v>
       </c>
+      <c r="K43" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="I44" s="2" t="s">
         <v>106</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="I45" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>108</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G46" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>79</v>
+        <v>60</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>110</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,88 +1561,88 @@
         <v>7</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>109</v>
+        <v>60</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="I47" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J47" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="J47" s="2" t="s">
-        <v>112</v>
+      <c r="K47" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G48" s="0" t="s">
-        <v>109</v>
+        <v>60</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="I48" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J48" s="2" t="s">
-        <v>114</v>
+      <c r="K48" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>109</v>
+        <v>60</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="I49" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J49" s="2" t="s">
-        <v>116</v>
+      <c r="K49" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="I50" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J50" s="2" t="s">
-        <v>118</v>
+      <c r="K50" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,65 +1650,65 @@
         <v>7</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>117</v>
+        <v>60</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>120</v>
+        <v>94</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>117</v>
+        <v>60</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="I52" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="J52" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J52" s="2" t="s">
-        <v>122</v>
+      <c r="K52" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>98</v>
+        <v>60</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>124</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>124</v>
+        <v>91</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1639,79 +1716,79 @@
         <v>7</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G54" s="0" t="s">
-        <v>123</v>
+        <v>60</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="I54" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J54" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J54" s="2" t="s">
-        <v>126</v>
+      <c r="K54" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I55" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I55" s="0" t="s">
         <v>128</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>128</v>
+        <v>104</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="I56" s="2" t="s">
         <v>130</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="G57" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>98</v>
+        <v>60</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,53 +1796,56 @@
         <v>7</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="G58" s="0" t="s">
-        <v>131</v>
+        <v>60</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>130</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="I58" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J58" s="2" t="s">
-        <v>134</v>
+      <c r="K58" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B60" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,30 +1853,33 @@
         <v>2</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>138</v>
+        <v>30</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>142</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>140</v>
+        <v>39</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,13 +1887,237 @@
         <v>1</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K69" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>